<commit_message>
first iteration of graphics. only first image creation
</commit_message>
<xml_diff>
--- a/Mass-model/Mass model/Masses.xlsx
+++ b/Mass-model/Mass model/Masses.xlsx
@@ -334,7 +334,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -347,7 +347,7 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -358,7 +358,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -369,7 +369,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -380,7 +380,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -391,7 +391,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -424,7 +424,7 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -435,7 +435,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -468,7 +468,7 @@
         <v>4</v>
       </c>
       <c r="C12">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -479,7 +479,7 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -490,7 +490,7 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -501,7 +501,7 @@
         <v>3</v>
       </c>
       <c r="C15">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -512,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="C16">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>